<commit_message>
update: overview and conclusion text in report
</commit_message>
<xml_diff>
--- a/Final-Report/HK251-DACN-ECOMMERCE-SHOP-WEBSITE/Images/plan2/plan2.xlsx
+++ b/Final-Report/HK251-DACN-ECOMMERCE-SHOP-WEBSITE/Images/plan2/plan2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BkEduDocs\Self_Study\Code\be-ecomerce-shop\Final-Report\HK251-DACN-ECOMMERCE-SHOP-WEBSITE\Images\plan2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{337D3FC2-60DA-44C4-AFB4-A3A5F87286BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5E863F-15D3-4E21-ADFF-3745F7F41269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{59DB41C4-A15A-4628-9519-025150C2E5C6}"/>
   </bookViews>
@@ -172,7 +172,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -195,16 +195,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -253,6 +286,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -570,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3006A49-778C-4A75-B7DE-1CD7B98FF519}">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -582,460 +624,461 @@
     <col min="12" max="12" width="75.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="2"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="20"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5" t="s">
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="12">
+      <c r="A4" s="10">
         <v>1</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="4">
         <f>DATE(2026,1,12)</f>
         <v>46034</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="7" t="s">
+      <c r="C4" s="4"/>
+      <c r="D4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="8" t="s">
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="12"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="12">
+      <c r="A10" s="10">
         <v>2</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="4">
         <f>B4+7</f>
         <v>46041</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="14">
+      <c r="A12" s="12">
         <v>3</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="13">
         <f>B10+7</f>
         <v>46048</v>
       </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="16" t="s">
+      <c r="C12" s="13"/>
+      <c r="D12" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="17" t="s">
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
     </row>
     <row r="13" spans="1:12" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="14">
+      <c r="A13" s="12">
         <v>4</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="13">
         <f t="shared" ref="B13:B24" si="0">B12+7</f>
         <v>46055</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="13">
+      <c r="A14" s="11">
         <v>5</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="4">
         <f t="shared" si="0"/>
         <v>46062</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="8" t="s">
+      <c r="C14" s="4"/>
+      <c r="D14" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="9" t="s">
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
     </row>
     <row r="15" spans="1:12" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="13">
+      <c r="A15" s="11">
         <v>6</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="4">
         <f t="shared" si="0"/>
         <v>46069</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="14">
+      <c r="A16" s="12">
         <v>7</v>
       </c>
-      <c r="B16" s="15">
+      <c r="B16" s="13">
         <f t="shared" si="0"/>
         <v>46076</v>
       </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="16" t="s">
+      <c r="C16" s="13"/>
+      <c r="D16" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="17" t="s">
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
     </row>
     <row r="17" spans="1:12" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="14">
+      <c r="A17" s="12">
         <v>8</v>
       </c>
-      <c r="B17" s="15">
+      <c r="B17" s="13">
         <f t="shared" si="0"/>
         <v>46083</v>
       </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="13">
+      <c r="A18" s="11">
         <v>9</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="4">
         <f t="shared" si="0"/>
         <v>46090</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="8" t="s">
+      <c r="C18" s="4"/>
+      <c r="D18" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8" t="s">
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
     </row>
     <row r="19" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="13">
+      <c r="A19" s="11">
         <v>10</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="4">
         <f t="shared" si="0"/>
         <v>46097</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="14">
+      <c r="A20" s="12">
         <v>11</v>
       </c>
-      <c r="B20" s="15">
+      <c r="B20" s="13">
         <f t="shared" si="0"/>
         <v>46104</v>
       </c>
-      <c r="C20" s="15"/>
-      <c r="D20" s="16" t="s">
+      <c r="C20" s="13"/>
+      <c r="D20" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="17" t="s">
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="17"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
     </row>
     <row r="21" spans="1:12" ht="69" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="14">
+      <c r="A21" s="12">
         <v>12</v>
       </c>
-      <c r="B21" s="15">
+      <c r="B21" s="13">
         <f t="shared" si="0"/>
         <v>46111</v>
       </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
     </row>
     <row r="22" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="14">
+      <c r="A22" s="12">
         <v>13</v>
       </c>
-      <c r="B22" s="15">
+      <c r="B22" s="13">
         <f t="shared" si="0"/>
         <v>46118</v>
       </c>
-      <c r="C22" s="15"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="13">
+      <c r="A23" s="11">
         <v>14</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="4">
         <f t="shared" si="0"/>
         <v>46125</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="11" t="s">
+      <c r="C23" s="4"/>
+      <c r="D23" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="9" t="s">
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
     </row>
     <row r="24" spans="1:12" ht="73.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="13">
+      <c r="A24" s="11">
         <v>15</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="4">
         <f t="shared" si="0"/>
         <v>46132</v>
       </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="36">
     <mergeCell ref="H23:L24"/>
+    <mergeCell ref="A1:L1"/>
     <mergeCell ref="D12:G13"/>
     <mergeCell ref="H12:L13"/>
     <mergeCell ref="D4:G11"/>
@@ -1066,7 +1109,6 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B18:C18"/>
-    <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B12:C12"/>

</xml_diff>